<commit_message>
update graphs for per month
</commit_message>
<xml_diff>
--- a/DinningData.xlsx
+++ b/DinningData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m.mughees/Desktop/DailyHours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843B1811-5FD8-F34D-A86F-E0032C3F0818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CFA9EB-AE6A-B245-B418-669AAF1F2D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DE998561-EBAC-6C45-B2D5-E0BAD589018C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{DE998561-EBAC-6C45-B2D5-E0BAD589018C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9694C3E-4676-5E45-83AA-01CD38B8296E}">
   <dimension ref="A1:H241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
-      <selection activeCell="I207" sqref="I207"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="H218" sqref="H218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.2"/>
@@ -661,7 +661,7 @@
         <v>4722.9799999999996</v>
       </c>
       <c r="F3" s="9">
-        <f t="shared" ref="F3:F20" si="0">E3*8.25</f>
+        <f t="shared" ref="F3:F13" si="0">E3*8.25</f>
         <v>38964.584999999999</v>
       </c>
       <c r="G3" s="1"/>
@@ -1002,12 +1002,10 @@
       <c r="D18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="13">
-        <v>1393.97</v>
-      </c>
+      <c r="E18" s="13"/>
       <c r="F18" s="8">
         <f t="shared" si="1"/>
-        <v>11500.252500000001</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1025,12 +1023,10 @@
       <c r="D19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="13">
-        <v>1469.16</v>
-      </c>
+      <c r="E19" s="13"/>
       <c r="F19" s="8">
         <f t="shared" si="1"/>
-        <v>12120.570000000002</v>
+        <v>0</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1048,12 +1044,10 @@
       <c r="D20" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="13">
-        <v>1325</v>
-      </c>
+      <c r="E20" s="13"/>
       <c r="F20" s="8">
         <f t="shared" si="1"/>
-        <v>10931.25</v>
+        <v>0</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1071,12 +1065,10 @@
       <c r="D21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="13">
-        <v>1242.47</v>
-      </c>
+      <c r="E21" s="13"/>
       <c r="F21" s="8">
-        <f t="shared" ref="F3:F66" si="2">E21*9.25</f>
-        <v>11492.8475</v>
+        <f t="shared" ref="F21:F49" si="2">E21*9.25</f>
+        <v>0</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1094,12 +1086,10 @@
       <c r="D22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="13">
-        <v>667.55</v>
-      </c>
+      <c r="E22" s="13"/>
       <c r="F22" s="8">
         <f t="shared" si="2"/>
-        <v>6174.8374999999996</v>
+        <v>0</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1117,12 +1107,10 @@
       <c r="D23" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="13">
-        <v>87.45</v>
-      </c>
+      <c r="E23" s="13"/>
       <c r="F23" s="8">
         <f t="shared" si="2"/>
-        <v>808.91250000000002</v>
+        <v>0</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1140,12 +1128,10 @@
       <c r="D24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="13">
-        <v>69.849999999999994</v>
-      </c>
+      <c r="E24" s="13"/>
       <c r="F24" s="8">
         <f t="shared" si="2"/>
-        <v>646.11249999999995</v>
+        <v>0</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1163,12 +1149,10 @@
       <c r="D25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="13">
-        <v>242.1</v>
-      </c>
+      <c r="E25" s="13"/>
       <c r="F25" s="8">
         <f t="shared" si="2"/>
-        <v>2239.4249999999997</v>
+        <v>0</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -1186,12 +1170,10 @@
       <c r="D26" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="12">
-        <v>2933.06</v>
-      </c>
+      <c r="E26" s="12"/>
       <c r="F26" s="9">
         <f t="shared" si="2"/>
-        <v>27130.805</v>
+        <v>0</v>
       </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -1209,12 +1191,10 @@
       <c r="D27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="12">
-        <v>2879.73</v>
-      </c>
+      <c r="E27" s="12"/>
       <c r="F27" s="9">
         <f>E27*9.25</f>
-        <v>26637.502499999999</v>
+        <v>0</v>
       </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -1232,12 +1212,10 @@
       <c r="D28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="12">
-        <v>2121.86</v>
-      </c>
+      <c r="E28" s="12"/>
       <c r="F28" s="9">
         <f t="shared" si="2"/>
-        <v>19627.205000000002</v>
+        <v>0</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -1255,12 +1233,10 @@
       <c r="D29" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E29" s="12">
-        <v>981.6</v>
-      </c>
+      <c r="E29" s="12"/>
       <c r="F29" s="9">
         <f t="shared" si="2"/>
-        <v>9079.8000000000011</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -2050,12 +2026,10 @@
       <c r="D66" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E66" s="13">
-        <v>640.91</v>
-      </c>
+      <c r="E66" s="13"/>
       <c r="F66" s="8">
         <f t="shared" si="4"/>
-        <v>5287.5074999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2071,12 +2045,10 @@
       <c r="D67" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E67" s="13">
-        <v>745.47</v>
-      </c>
+      <c r="E67" s="13"/>
       <c r="F67" s="8">
         <f t="shared" si="4"/>
-        <v>6150.1275000000005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -2092,12 +2064,10 @@
       <c r="D68" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E68" s="13">
-        <v>645.36</v>
-      </c>
+      <c r="E68" s="13"/>
       <c r="F68" s="8">
         <f t="shared" si="4"/>
-        <v>5324.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -2113,12 +2083,10 @@
       <c r="D69" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="13">
-        <v>673.74</v>
-      </c>
+      <c r="E69" s="13"/>
       <c r="F69" s="8">
-        <f t="shared" ref="F67:F130" si="5">E69*9.25</f>
-        <v>6232.0950000000003</v>
+        <f t="shared" ref="F69:F130" si="5">E69*9.25</f>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -2134,12 +2102,10 @@
       <c r="D70" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E70" s="13">
-        <v>315.25</v>
-      </c>
+      <c r="E70" s="13"/>
       <c r="F70" s="8">
         <f t="shared" si="5"/>
-        <v>2916.0625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2155,9 +2121,7 @@
       <c r="D71" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E71" s="13">
-        <v>0</v>
-      </c>
+      <c r="E71" s="13"/>
       <c r="F71" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2176,9 +2140,7 @@
       <c r="D72" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E72" s="13">
-        <v>0</v>
-      </c>
+      <c r="E72" s="13"/>
       <c r="F72" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2197,12 +2159,10 @@
       <c r="D73" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E73" s="13">
-        <v>14.3</v>
-      </c>
+      <c r="E73" s="13"/>
       <c r="F73" s="8">
         <f t="shared" si="5"/>
-        <v>132.27500000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2218,12 +2178,10 @@
       <c r="D74" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E74" s="12">
-        <v>1106.45</v>
-      </c>
+      <c r="E74" s="12"/>
       <c r="F74" s="9">
         <f t="shared" si="5"/>
-        <v>10234.6625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2239,12 +2197,10 @@
       <c r="D75" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E75" s="12">
-        <v>1035.07</v>
-      </c>
+      <c r="E75" s="12"/>
       <c r="F75" s="9">
         <f t="shared" si="5"/>
-        <v>9574.3974999999991</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2260,12 +2216,10 @@
       <c r="D76" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E76" s="12">
-        <v>832.44</v>
-      </c>
+      <c r="E76" s="12"/>
       <c r="F76" s="9">
         <f t="shared" si="5"/>
-        <v>7700.0700000000006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2281,12 +2235,10 @@
       <c r="D77" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E77" s="12">
-        <v>462.07</v>
-      </c>
+      <c r="E77" s="12"/>
       <c r="F77" s="9">
         <f t="shared" si="5"/>
-        <v>4274.1475</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -3058,12 +3010,10 @@
       <c r="D114" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E114" s="13">
-        <v>436.52</v>
-      </c>
+      <c r="E114" s="13"/>
       <c r="F114" s="8">
         <f t="shared" si="7"/>
-        <v>3601.29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -3079,12 +3029,10 @@
       <c r="D115" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E115" s="13">
-        <v>561.79</v>
-      </c>
+      <c r="E115" s="13"/>
       <c r="F115" s="8">
         <f t="shared" si="7"/>
-        <v>4634.7674999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -3100,12 +3048,10 @@
       <c r="D116" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E116" s="13">
-        <v>583.91</v>
-      </c>
+      <c r="E116" s="13"/>
       <c r="F116" s="8">
         <f t="shared" si="7"/>
-        <v>4817.2574999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -3121,12 +3067,10 @@
       <c r="D117" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E117" s="13">
-        <v>516.86</v>
-      </c>
+      <c r="E117" s="13"/>
       <c r="F117" s="8">
         <f t="shared" si="5"/>
-        <v>4780.9549999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -3142,12 +3086,10 @@
       <c r="D118" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E118" s="13">
-        <v>263.36</v>
-      </c>
+      <c r="E118" s="13"/>
       <c r="F118" s="8">
         <f t="shared" si="5"/>
-        <v>2436.08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -3163,9 +3105,7 @@
       <c r="D119" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E119" s="13">
-        <v>0</v>
-      </c>
+      <c r="E119" s="13"/>
       <c r="F119" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3184,9 +3124,7 @@
       <c r="D120" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E120" s="13">
-        <v>0</v>
-      </c>
+      <c r="E120" s="13"/>
       <c r="F120" s="8">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -3205,12 +3143,10 @@
       <c r="D121" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E121" s="13">
-        <v>33.82</v>
-      </c>
+      <c r="E121" s="13"/>
       <c r="F121" s="8">
         <f t="shared" si="5"/>
-        <v>312.83499999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -3226,12 +3162,10 @@
       <c r="D122" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E122" s="12">
-        <v>721.13</v>
-      </c>
+      <c r="E122" s="12"/>
       <c r="F122" s="9">
         <f t="shared" si="5"/>
-        <v>6670.4525000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3247,12 +3181,10 @@
       <c r="D123" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E123" s="12">
-        <v>755.56</v>
-      </c>
+      <c r="E123" s="12"/>
       <c r="F123" s="9">
         <f t="shared" si="5"/>
-        <v>6988.9299999999994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -3268,12 +3200,10 @@
       <c r="D124" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E124" s="12">
-        <v>604.24</v>
-      </c>
+      <c r="E124" s="12"/>
       <c r="F124" s="9">
         <f t="shared" si="5"/>
-        <v>5589.22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -3289,12 +3219,10 @@
       <c r="D125" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E125" s="12">
-        <v>312.41000000000003</v>
-      </c>
+      <c r="E125" s="12"/>
       <c r="F125" s="9">
         <f t="shared" si="5"/>
-        <v>2889.7925</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -3419,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="F131" s="9">
-        <f t="shared" ref="F131:F194" si="8">E131*9.25</f>
+        <f t="shared" ref="F131:F193" si="8">E131*9.25</f>
         <v>0</v>
       </c>
     </row>
@@ -4066,12 +3994,10 @@
       <c r="D162" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E162" s="6">
-        <v>174.43</v>
-      </c>
+      <c r="E162" s="6"/>
       <c r="F162" s="8">
         <f t="shared" si="10"/>
-        <v>1439.0475000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
@@ -4087,12 +4013,10 @@
       <c r="D163" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E163" s="6">
-        <v>271.83</v>
-      </c>
+      <c r="E163" s="6"/>
       <c r="F163" s="8">
         <f t="shared" si="10"/>
-        <v>2242.5974999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
@@ -4108,12 +4032,10 @@
       <c r="D164" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E164" s="6">
-        <v>223.21</v>
-      </c>
+      <c r="E164" s="6"/>
       <c r="F164" s="8">
         <f t="shared" si="10"/>
-        <v>1841.4825000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
@@ -4129,12 +4051,10 @@
       <c r="D165" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E165" s="6">
-        <v>240.16</v>
-      </c>
+      <c r="E165" s="6"/>
       <c r="F165" s="8">
         <f t="shared" si="8"/>
-        <v>2221.48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
@@ -4150,12 +4070,10 @@
       <c r="D166" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E166" s="6">
-        <v>123.89</v>
-      </c>
+      <c r="E166" s="6"/>
       <c r="F166" s="8">
         <f t="shared" si="8"/>
-        <v>1145.9825000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
@@ -4171,9 +4089,7 @@
       <c r="D167" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E167" s="6">
-        <v>0</v>
-      </c>
+      <c r="E167" s="6"/>
       <c r="F167" s="8">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -4192,9 +4108,7 @@
       <c r="D168" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E168" s="6">
-        <v>0</v>
-      </c>
+      <c r="E168" s="6"/>
       <c r="F168" s="8">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -4213,12 +4127,10 @@
       <c r="D169" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E169" s="6">
-        <v>3.83</v>
-      </c>
+      <c r="E169" s="6"/>
       <c r="F169" s="8">
         <f t="shared" si="8"/>
-        <v>35.427500000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
@@ -4234,12 +4146,10 @@
       <c r="D170" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E170" s="7">
-        <v>251.17</v>
-      </c>
+      <c r="E170" s="7"/>
       <c r="F170" s="9">
         <f t="shared" si="8"/>
-        <v>2323.3224999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
@@ -4255,12 +4165,10 @@
       <c r="D171" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E171" s="7">
-        <v>247.68</v>
-      </c>
+      <c r="E171" s="7"/>
       <c r="F171" s="9">
         <f t="shared" si="8"/>
-        <v>2291.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
@@ -4276,12 +4184,10 @@
       <c r="D172" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E172" s="7">
-        <v>197.65</v>
-      </c>
+      <c r="E172" s="7"/>
       <c r="F172" s="9">
         <f t="shared" si="8"/>
-        <v>1828.2625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -4297,12 +4203,10 @@
       <c r="D173" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E173" s="7">
-        <v>102.21</v>
-      </c>
+      <c r="E173" s="7"/>
       <c r="F173" s="9">
         <f t="shared" si="8"/>
-        <v>945.4425</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
@@ -5074,12 +4978,10 @@
       <c r="D210" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E210" s="6">
-        <v>22.06</v>
-      </c>
+      <c r="E210" s="6"/>
       <c r="F210" s="8">
         <f t="shared" si="12"/>
-        <v>181.99499999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
@@ -5095,12 +4997,10 @@
       <c r="D211" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E211" s="6">
-        <v>72.47</v>
-      </c>
+      <c r="E211" s="6"/>
       <c r="F211" s="8">
         <f t="shared" si="12"/>
-        <v>597.87749999999994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
@@ -5116,12 +5016,10 @@
       <c r="D212" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E212" s="6">
-        <v>52.08</v>
-      </c>
+      <c r="E212" s="6"/>
       <c r="F212" s="8">
         <f t="shared" si="12"/>
-        <v>429.65999999999997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
@@ -5137,12 +5035,10 @@
       <c r="D213" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E213" s="6">
-        <v>61.2</v>
-      </c>
+      <c r="E213" s="6"/>
       <c r="F213" s="8">
-        <f t="shared" ref="F195:F241" si="13">E213*9.25</f>
-        <v>566.1</v>
+        <f t="shared" ref="F213:F241" si="13">E213*9.25</f>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
@@ -5158,12 +5054,10 @@
       <c r="D214" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E214" s="6">
-        <v>32.54</v>
-      </c>
+      <c r="E214" s="6"/>
       <c r="F214" s="8">
         <f t="shared" si="13"/>
-        <v>300.995</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.25">
@@ -5179,12 +5073,10 @@
       <c r="D215" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E215" s="6">
-        <v>32</v>
-      </c>
+      <c r="E215" s="6"/>
       <c r="F215" s="8">
         <f t="shared" si="13"/>
-        <v>296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
@@ -5200,9 +5092,7 @@
       <c r="D216" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E216" s="6">
-        <v>0</v>
-      </c>
+      <c r="E216" s="6"/>
       <c r="F216" s="8">
         <f t="shared" si="13"/>
         <v>0</v>
@@ -5221,12 +5111,10 @@
       <c r="D217" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E217" s="6">
-        <v>5.93</v>
-      </c>
+      <c r="E217" s="6"/>
       <c r="F217" s="8">
         <f t="shared" si="13"/>
-        <v>54.852499999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.25">
@@ -5242,12 +5130,10 @@
       <c r="D218" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E218" s="7">
-        <v>178.53</v>
-      </c>
+      <c r="E218" s="7"/>
       <c r="F218" s="9">
         <f t="shared" si="13"/>
-        <v>1651.4024999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
@@ -5263,12 +5149,10 @@
       <c r="D219" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E219" s="7">
-        <v>228.9</v>
-      </c>
+      <c r="E219" s="7"/>
       <c r="F219" s="9">
         <f t="shared" si="13"/>
-        <v>2117.3250000000003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.25">
@@ -5284,12 +5168,10 @@
       <c r="D220" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E220" s="7">
-        <v>188.95</v>
-      </c>
+      <c r="E220" s="7"/>
       <c r="F220" s="9">
         <f t="shared" si="13"/>
-        <v>1747.7874999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.25">
@@ -5305,12 +5187,10 @@
       <c r="D221" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E221" s="7">
-        <v>130.63999999999999</v>
-      </c>
+      <c r="E221" s="7"/>
       <c r="F221" s="9">
         <f t="shared" si="13"/>
-        <v>1208.4199999999998</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
linear regression on the data
</commit_message>
<xml_diff>
--- a/DinningData.xlsx
+++ b/DinningData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m.mughees/Desktop/DailyHours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7561C47-8446-C543-9B92-70D3C03B8E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F164DC42-F400-D340-8D89-149C526759DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DE998561-EBAC-6C45-B2D5-E0BAD589018C}"/>
+    <workbookView xWindow="16040" yWindow="-26720" windowWidth="28800" windowHeight="16280" xr2:uid="{DE998561-EBAC-6C45-B2D5-E0BAD589018C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>DEP</t>
   </si>
@@ -45,18 +45,6 @@
   </si>
   <si>
     <t>Month</t>
-  </si>
-  <si>
-    <t>Fall</t>
-  </si>
-  <si>
-    <t>J-Term</t>
-  </si>
-  <si>
-    <t>Spring</t>
-  </si>
-  <si>
-    <t>Summer</t>
   </si>
   <si>
     <t>Hours</t>
@@ -541,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9694C3E-4676-5E45-83AA-01CD38B8296E}">
   <dimension ref="A1:T241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="L245" sqref="L245"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K230" sqref="K230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.2"/>
@@ -567,13 +555,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -582,8 +570,8 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>3</v>
+      <c r="B2" s="4">
+        <v>1</v>
       </c>
       <c r="C2" s="5">
         <v>9</v>
@@ -605,8 +593,8 @@
       <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>3</v>
+      <c r="B3" s="4">
+        <v>1</v>
       </c>
       <c r="C3" s="5">
         <v>10</v>
@@ -628,8 +616,8 @@
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>3</v>
+      <c r="B4" s="4">
+        <v>1</v>
       </c>
       <c r="C4" s="5">
         <v>11</v>
@@ -651,8 +639,8 @@
       <c r="A5" s="4">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>3</v>
+      <c r="B5" s="4">
+        <v>1</v>
       </c>
       <c r="C5" s="5">
         <v>12</v>
@@ -674,8 +662,8 @@
       <c r="A6" s="4">
         <v>1</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
+      <c r="B6" s="4">
+        <v>2</v>
       </c>
       <c r="C6" s="5">
         <v>1</v>
@@ -697,8 +685,8 @@
       <c r="A7" s="4">
         <v>1</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>5</v>
+      <c r="B7" s="4">
+        <v>3</v>
       </c>
       <c r="C7" s="5">
         <v>2</v>
@@ -720,8 +708,8 @@
       <c r="A8" s="4">
         <v>1</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>5</v>
+      <c r="B8" s="4">
+        <v>3</v>
       </c>
       <c r="C8" s="5">
         <v>3</v>
@@ -743,8 +731,8 @@
       <c r="A9" s="4">
         <v>1</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>5</v>
+      <c r="B9" s="4">
+        <v>3</v>
       </c>
       <c r="C9" s="5">
         <v>4</v>
@@ -766,8 +754,8 @@
       <c r="A10" s="4">
         <v>1</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>5</v>
+      <c r="B10" s="4">
+        <v>3</v>
       </c>
       <c r="C10" s="5">
         <v>5</v>
@@ -789,8 +777,8 @@
       <c r="A11" s="4">
         <v>1</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>6</v>
+      <c r="B11" s="4">
+        <v>4</v>
       </c>
       <c r="C11" s="5">
         <v>6</v>
@@ -812,8 +800,8 @@
       <c r="A12" s="4">
         <v>1</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>6</v>
+      <c r="B12" s="4">
+        <v>4</v>
       </c>
       <c r="C12" s="5">
         <v>7</v>
@@ -835,8 +823,8 @@
       <c r="A13" s="4">
         <v>1</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>6</v>
+      <c r="B13" s="4">
+        <v>4</v>
       </c>
       <c r="C13" s="5">
         <v>8</v>
@@ -858,8 +846,8 @@
       <c r="A14" s="2">
         <v>1</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
+      <c r="B14" s="2">
+        <v>1</v>
       </c>
       <c r="C14" s="3">
         <v>9</v>
@@ -881,8 +869,8 @@
       <c r="A15" s="2">
         <v>1</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>3</v>
+      <c r="B15" s="2">
+        <v>1</v>
       </c>
       <c r="C15" s="3">
         <v>10</v>
@@ -904,8 +892,8 @@
       <c r="A16" s="2">
         <v>1</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>3</v>
+      <c r="B16" s="2">
+        <v>1</v>
       </c>
       <c r="C16" s="3">
         <v>11</v>
@@ -927,8 +915,8 @@
       <c r="A17" s="2">
         <v>1</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>3</v>
+      <c r="B17" s="2">
+        <v>1</v>
       </c>
       <c r="C17" s="3">
         <v>12</v>
@@ -950,8 +938,8 @@
       <c r="A18" s="2">
         <v>1</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>4</v>
+      <c r="B18" s="2">
+        <v>2</v>
       </c>
       <c r="C18" s="3">
         <v>1</v>
@@ -971,8 +959,8 @@
       <c r="A19" s="2">
         <v>1</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
+      <c r="B19" s="2">
+        <v>3</v>
       </c>
       <c r="C19" s="3">
         <v>2</v>
@@ -992,8 +980,8 @@
       <c r="A20" s="2">
         <v>1</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
+      <c r="B20" s="2">
+        <v>3</v>
       </c>
       <c r="C20" s="3">
         <v>3</v>
@@ -1013,8 +1001,8 @@
       <c r="A21" s="2">
         <v>1</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
+      <c r="B21" s="2">
+        <v>3</v>
       </c>
       <c r="C21" s="3">
         <v>4</v>
@@ -1028,14 +1016,13 @@
         <v>0</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>1</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>5</v>
+      <c r="B22" s="2">
+        <v>3</v>
       </c>
       <c r="C22" s="3">
         <v>5</v>
@@ -1055,8 +1042,8 @@
       <c r="A23" s="2">
         <v>1</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>6</v>
+      <c r="B23" s="2">
+        <v>4</v>
       </c>
       <c r="C23" s="3">
         <v>6</v>
@@ -1076,8 +1063,8 @@
       <c r="A24" s="2">
         <v>1</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>6</v>
+      <c r="B24" s="2">
+        <v>4</v>
       </c>
       <c r="C24" s="3">
         <v>7</v>
@@ -1104,8 +1091,8 @@
       <c r="A25" s="2">
         <v>1</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>6</v>
+      <c r="B25" s="2">
+        <v>4</v>
       </c>
       <c r="C25" s="3">
         <v>8</v>
@@ -1132,8 +1119,8 @@
       <c r="A26" s="4">
         <v>1</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>3</v>
+      <c r="B26" s="4">
+        <v>1</v>
       </c>
       <c r="C26" s="5">
         <v>9</v>
@@ -1160,8 +1147,8 @@
       <c r="A27" s="4">
         <v>1</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>3</v>
+      <c r="B27" s="4">
+        <v>1</v>
       </c>
       <c r="C27" s="5">
         <v>10</v>
@@ -1188,8 +1175,8 @@
       <c r="A28" s="4">
         <v>1</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>3</v>
+      <c r="B28" s="4">
+        <v>1</v>
       </c>
       <c r="C28" s="5">
         <v>11</v>
@@ -1216,8 +1203,8 @@
       <c r="A29" s="4">
         <v>1</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>3</v>
+      <c r="B29" s="4">
+        <v>1</v>
       </c>
       <c r="C29" s="5">
         <v>12</v>
@@ -1244,8 +1231,8 @@
       <c r="A30" s="4">
         <v>1</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>4</v>
+      <c r="B30" s="4">
+        <v>2</v>
       </c>
       <c r="C30" s="5">
         <v>1</v>
@@ -1274,8 +1261,8 @@
       <c r="A31" s="4">
         <v>1</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>5</v>
+      <c r="B31" s="4">
+        <v>3</v>
       </c>
       <c r="C31" s="5">
         <v>2</v>
@@ -1304,8 +1291,8 @@
       <c r="A32" s="4">
         <v>1</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>5</v>
+      <c r="B32" s="4">
+        <v>3</v>
       </c>
       <c r="C32" s="5">
         <v>3</v>
@@ -1334,8 +1321,8 @@
       <c r="A33" s="4">
         <v>1</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>5</v>
+      <c r="B33" s="4">
+        <v>3</v>
       </c>
       <c r="C33" s="5">
         <v>4</v>
@@ -1364,8 +1351,8 @@
       <c r="A34" s="4">
         <v>1</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>5</v>
+      <c r="B34" s="4">
+        <v>3</v>
       </c>
       <c r="C34" s="5">
         <v>5</v>
@@ -1394,8 +1381,8 @@
       <c r="A35" s="4">
         <v>1</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>6</v>
+      <c r="B35" s="4">
+        <v>4</v>
       </c>
       <c r="C35" s="5">
         <v>6</v>
@@ -1424,8 +1411,8 @@
       <c r="A36" s="4">
         <v>1</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>6</v>
+      <c r="B36" s="4">
+        <v>4</v>
       </c>
       <c r="C36" s="5">
         <v>7</v>
@@ -1448,8 +1435,8 @@
       <c r="A37" s="4">
         <v>1</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>6</v>
+      <c r="B37" s="4">
+        <v>4</v>
       </c>
       <c r="C37" s="5">
         <v>8</v>
@@ -1472,8 +1459,8 @@
       <c r="A38" s="2">
         <v>1</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>3</v>
+      <c r="B38" s="2">
+        <v>1</v>
       </c>
       <c r="C38" s="3">
         <v>9</v>
@@ -1494,8 +1481,8 @@
       <c r="A39" s="2">
         <v>1</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>3</v>
+      <c r="B39" s="2">
+        <v>1</v>
       </c>
       <c r="C39" s="3">
         <v>10</v>
@@ -1515,8 +1502,8 @@
       <c r="A40" s="2">
         <v>1</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>3</v>
+      <c r="B40" s="2">
+        <v>1</v>
       </c>
       <c r="C40" s="3">
         <v>11</v>
@@ -1536,8 +1523,8 @@
       <c r="A41" s="2">
         <v>1</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>3</v>
+      <c r="B41" s="2">
+        <v>1</v>
       </c>
       <c r="C41" s="3">
         <v>12</v>
@@ -1557,8 +1544,8 @@
       <c r="A42" s="2">
         <v>1</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>4</v>
+      <c r="B42" s="2">
+        <v>2</v>
       </c>
       <c r="C42" s="3">
         <v>1</v>
@@ -1578,8 +1565,8 @@
       <c r="A43" s="2">
         <v>1</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>5</v>
+      <c r="B43" s="2">
+        <v>3</v>
       </c>
       <c r="C43" s="3">
         <v>2</v>
@@ -1599,8 +1586,8 @@
       <c r="A44" s="2">
         <v>1</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>5</v>
+      <c r="B44" s="2">
+        <v>3</v>
       </c>
       <c r="C44" s="3">
         <v>3</v>
@@ -1620,8 +1607,8 @@
       <c r="A45" s="2">
         <v>1</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>5</v>
+      <c r="B45" s="2">
+        <v>3</v>
       </c>
       <c r="C45" s="3">
         <v>4</v>
@@ -1641,8 +1628,8 @@
       <c r="A46" s="2">
         <v>1</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>5</v>
+      <c r="B46" s="2">
+        <v>3</v>
       </c>
       <c r="C46" s="3">
         <v>5</v>
@@ -1662,8 +1649,8 @@
       <c r="A47" s="2">
         <v>1</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>6</v>
+      <c r="B47" s="2">
+        <v>4</v>
       </c>
       <c r="C47" s="3">
         <v>6</v>
@@ -1683,8 +1670,8 @@
       <c r="A48" s="2">
         <v>1</v>
       </c>
-      <c r="B48" s="2" t="s">
-        <v>6</v>
+      <c r="B48" s="2">
+        <v>4</v>
       </c>
       <c r="C48" s="3">
         <v>7</v>
@@ -1704,8 +1691,8 @@
       <c r="A49" s="2">
         <v>1</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>6</v>
+      <c r="B49" s="2">
+        <v>4</v>
       </c>
       <c r="C49" s="3">
         <v>8</v>
@@ -1725,8 +1712,8 @@
       <c r="A50" s="4">
         <v>2</v>
       </c>
-      <c r="B50" s="4" t="s">
-        <v>3</v>
+      <c r="B50" s="4">
+        <v>1</v>
       </c>
       <c r="C50" s="5">
         <v>9</v>
@@ -1746,8 +1733,8 @@
       <c r="A51" s="4">
         <v>2</v>
       </c>
-      <c r="B51" s="4" t="s">
-        <v>3</v>
+      <c r="B51" s="4">
+        <v>1</v>
       </c>
       <c r="C51" s="5">
         <v>10</v>
@@ -1767,8 +1754,8 @@
       <c r="A52" s="4">
         <v>2</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>3</v>
+      <c r="B52" s="4">
+        <v>1</v>
       </c>
       <c r="C52" s="5">
         <v>11</v>
@@ -1788,8 +1775,8 @@
       <c r="A53" s="4">
         <v>2</v>
       </c>
-      <c r="B53" s="4" t="s">
-        <v>3</v>
+      <c r="B53" s="4">
+        <v>1</v>
       </c>
       <c r="C53" s="5">
         <v>12</v>
@@ -1809,8 +1796,8 @@
       <c r="A54" s="4">
         <v>2</v>
       </c>
-      <c r="B54" s="4" t="s">
-        <v>4</v>
+      <c r="B54" s="4">
+        <v>2</v>
       </c>
       <c r="C54" s="5">
         <v>1</v>
@@ -1830,8 +1817,8 @@
       <c r="A55" s="4">
         <v>2</v>
       </c>
-      <c r="B55" s="4" t="s">
-        <v>5</v>
+      <c r="B55" s="4">
+        <v>3</v>
       </c>
       <c r="C55" s="5">
         <v>2</v>
@@ -1851,8 +1838,8 @@
       <c r="A56" s="4">
         <v>2</v>
       </c>
-      <c r="B56" s="4" t="s">
-        <v>5</v>
+      <c r="B56" s="4">
+        <v>3</v>
       </c>
       <c r="C56" s="5">
         <v>3</v>
@@ -1872,8 +1859,8 @@
       <c r="A57" s="4">
         <v>2</v>
       </c>
-      <c r="B57" s="4" t="s">
-        <v>5</v>
+      <c r="B57" s="4">
+        <v>3</v>
       </c>
       <c r="C57" s="5">
         <v>4</v>
@@ -1893,8 +1880,8 @@
       <c r="A58" s="4">
         <v>2</v>
       </c>
-      <c r="B58" s="4" t="s">
-        <v>5</v>
+      <c r="B58" s="4">
+        <v>3</v>
       </c>
       <c r="C58" s="5">
         <v>5</v>
@@ -1914,8 +1901,8 @@
       <c r="A59" s="4">
         <v>2</v>
       </c>
-      <c r="B59" s="4" t="s">
-        <v>6</v>
+      <c r="B59" s="4">
+        <v>4</v>
       </c>
       <c r="C59" s="5">
         <v>6</v>
@@ -1935,8 +1922,8 @@
       <c r="A60" s="4">
         <v>2</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>6</v>
+      <c r="B60" s="4">
+        <v>4</v>
       </c>
       <c r="C60" s="5">
         <v>7</v>
@@ -1956,8 +1943,8 @@
       <c r="A61" s="4">
         <v>2</v>
       </c>
-      <c r="B61" s="4" t="s">
-        <v>6</v>
+      <c r="B61" s="4">
+        <v>4</v>
       </c>
       <c r="C61" s="5">
         <v>8</v>
@@ -1977,8 +1964,8 @@
       <c r="A62" s="2">
         <v>2</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>3</v>
+      <c r="B62" s="2">
+        <v>1</v>
       </c>
       <c r="C62" s="3">
         <v>9</v>
@@ -1998,8 +1985,8 @@
       <c r="A63" s="2">
         <v>2</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>3</v>
+      <c r="B63" s="2">
+        <v>1</v>
       </c>
       <c r="C63" s="3">
         <v>10</v>
@@ -2019,8 +2006,8 @@
       <c r="A64" s="2">
         <v>2</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>3</v>
+      <c r="B64" s="2">
+        <v>1</v>
       </c>
       <c r="C64" s="3">
         <v>11</v>
@@ -2040,8 +2027,8 @@
       <c r="A65" s="2">
         <v>2</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>3</v>
+      <c r="B65" s="2">
+        <v>1</v>
       </c>
       <c r="C65" s="3">
         <v>12</v>
@@ -2061,8 +2048,8 @@
       <c r="A66" s="2">
         <v>2</v>
       </c>
-      <c r="B66" s="2" t="s">
-        <v>4</v>
+      <c r="B66" s="2">
+        <v>2</v>
       </c>
       <c r="C66" s="3">
         <v>1</v>
@@ -2080,8 +2067,8 @@
       <c r="A67" s="2">
         <v>2</v>
       </c>
-      <c r="B67" s="2" t="s">
-        <v>5</v>
+      <c r="B67" s="2">
+        <v>3</v>
       </c>
       <c r="C67" s="3">
         <v>2</v>
@@ -2099,8 +2086,8 @@
       <c r="A68" s="2">
         <v>2</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>5</v>
+      <c r="B68" s="2">
+        <v>3</v>
       </c>
       <c r="C68" s="3">
         <v>3</v>
@@ -2118,8 +2105,8 @@
       <c r="A69" s="2">
         <v>2</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>5</v>
+      <c r="B69" s="2">
+        <v>3</v>
       </c>
       <c r="C69" s="3">
         <v>4</v>
@@ -2144,8 +2131,8 @@
       <c r="A70" s="2">
         <v>2</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>5</v>
+      <c r="B70" s="2">
+        <v>3</v>
       </c>
       <c r="C70" s="3">
         <v>5</v>
@@ -2170,8 +2157,8 @@
       <c r="A71" s="2">
         <v>2</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>6</v>
+      <c r="B71" s="2">
+        <v>4</v>
       </c>
       <c r="C71" s="3">
         <v>6</v>
@@ -2196,8 +2183,8 @@
       <c r="A72" s="2">
         <v>2</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>6</v>
+      <c r="B72" s="2">
+        <v>4</v>
       </c>
       <c r="C72" s="3">
         <v>7</v>
@@ -2222,8 +2209,8 @@
       <c r="A73" s="2">
         <v>2</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>6</v>
+      <c r="B73" s="2">
+        <v>4</v>
       </c>
       <c r="C73" s="3">
         <v>8</v>
@@ -2248,8 +2235,8 @@
       <c r="A74" s="4">
         <v>2</v>
       </c>
-      <c r="B74" s="4" t="s">
-        <v>3</v>
+      <c r="B74" s="4">
+        <v>1</v>
       </c>
       <c r="C74" s="5">
         <v>9</v>
@@ -2274,8 +2261,8 @@
       <c r="A75" s="4">
         <v>2</v>
       </c>
-      <c r="B75" s="4" t="s">
-        <v>3</v>
+      <c r="B75" s="4">
+        <v>1</v>
       </c>
       <c r="C75" s="5">
         <v>10</v>
@@ -2300,8 +2287,8 @@
       <c r="A76" s="4">
         <v>2</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>3</v>
+      <c r="B76" s="4">
+        <v>1</v>
       </c>
       <c r="C76" s="5">
         <v>11</v>
@@ -2326,8 +2313,8 @@
       <c r="A77" s="4">
         <v>2</v>
       </c>
-      <c r="B77" s="4" t="s">
-        <v>3</v>
+      <c r="B77" s="4">
+        <v>1</v>
       </c>
       <c r="C77" s="5">
         <v>12</v>
@@ -2352,8 +2339,8 @@
       <c r="A78" s="4">
         <v>2</v>
       </c>
-      <c r="B78" s="4" t="s">
-        <v>4</v>
+      <c r="B78" s="4">
+        <v>2</v>
       </c>
       <c r="C78" s="5">
         <v>1</v>
@@ -2380,8 +2367,8 @@
       <c r="A79" s="4">
         <v>2</v>
       </c>
-      <c r="B79" s="4" t="s">
-        <v>5</v>
+      <c r="B79" s="4">
+        <v>3</v>
       </c>
       <c r="C79" s="5">
         <v>2</v>
@@ -2408,8 +2395,8 @@
       <c r="A80" s="4">
         <v>2</v>
       </c>
-      <c r="B80" s="4" t="s">
-        <v>5</v>
+      <c r="B80" s="4">
+        <v>3</v>
       </c>
       <c r="C80" s="5">
         <v>3</v>
@@ -2436,8 +2423,8 @@
       <c r="A81" s="4">
         <v>2</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>5</v>
+      <c r="B81" s="4">
+        <v>3</v>
       </c>
       <c r="C81" s="5">
         <v>4</v>
@@ -2457,8 +2444,8 @@
       <c r="A82" s="4">
         <v>2</v>
       </c>
-      <c r="B82" s="4" t="s">
-        <v>5</v>
+      <c r="B82" s="4">
+        <v>3</v>
       </c>
       <c r="C82" s="5">
         <v>5</v>
@@ -2478,8 +2465,8 @@
       <c r="A83" s="4">
         <v>2</v>
       </c>
-      <c r="B83" s="4" t="s">
-        <v>6</v>
+      <c r="B83" s="4">
+        <v>4</v>
       </c>
       <c r="C83" s="5">
         <v>6</v>
@@ -2499,8 +2486,8 @@
       <c r="A84" s="4">
         <v>2</v>
       </c>
-      <c r="B84" s="4" t="s">
-        <v>6</v>
+      <c r="B84" s="4">
+        <v>4</v>
       </c>
       <c r="C84" s="5">
         <v>7</v>
@@ -2520,8 +2507,8 @@
       <c r="A85" s="4">
         <v>2</v>
       </c>
-      <c r="B85" s="4" t="s">
-        <v>6</v>
+      <c r="B85" s="4">
+        <v>4</v>
       </c>
       <c r="C85" s="5">
         <v>8</v>
@@ -2541,8 +2528,8 @@
       <c r="A86" s="2">
         <v>2</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>3</v>
+      <c r="B86" s="2">
+        <v>1</v>
       </c>
       <c r="C86" s="3">
         <v>9</v>
@@ -2562,8 +2549,8 @@
       <c r="A87" s="2">
         <v>2</v>
       </c>
-      <c r="B87" s="2" t="s">
-        <v>3</v>
+      <c r="B87" s="2">
+        <v>1</v>
       </c>
       <c r="C87" s="3">
         <v>10</v>
@@ -2583,8 +2570,8 @@
       <c r="A88" s="2">
         <v>2</v>
       </c>
-      <c r="B88" s="2" t="s">
-        <v>3</v>
+      <c r="B88" s="2">
+        <v>1</v>
       </c>
       <c r="C88" s="3">
         <v>11</v>
@@ -2604,8 +2591,8 @@
       <c r="A89" s="2">
         <v>2</v>
       </c>
-      <c r="B89" s="2" t="s">
-        <v>3</v>
+      <c r="B89" s="2">
+        <v>1</v>
       </c>
       <c r="C89" s="3">
         <v>12</v>
@@ -2625,8 +2612,8 @@
       <c r="A90" s="2">
         <v>2</v>
       </c>
-      <c r="B90" s="2" t="s">
-        <v>4</v>
+      <c r="B90" s="2">
+        <v>2</v>
       </c>
       <c r="C90" s="3">
         <v>1</v>
@@ -2646,8 +2633,8 @@
       <c r="A91" s="2">
         <v>2</v>
       </c>
-      <c r="B91" s="2" t="s">
-        <v>5</v>
+      <c r="B91" s="2">
+        <v>3</v>
       </c>
       <c r="C91" s="3">
         <v>2</v>
@@ -2667,8 +2654,8 @@
       <c r="A92" s="2">
         <v>2</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>5</v>
+      <c r="B92" s="2">
+        <v>3</v>
       </c>
       <c r="C92" s="3">
         <v>3</v>
@@ -2688,8 +2675,8 @@
       <c r="A93" s="2">
         <v>2</v>
       </c>
-      <c r="B93" s="2" t="s">
-        <v>5</v>
+      <c r="B93" s="2">
+        <v>3</v>
       </c>
       <c r="C93" s="3">
         <v>4</v>
@@ -2709,8 +2696,8 @@
       <c r="A94" s="2">
         <v>2</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>5</v>
+      <c r="B94" s="2">
+        <v>3</v>
       </c>
       <c r="C94" s="3">
         <v>5</v>
@@ -2730,8 +2717,8 @@
       <c r="A95" s="2">
         <v>2</v>
       </c>
-      <c r="B95" s="2" t="s">
-        <v>6</v>
+      <c r="B95" s="2">
+        <v>4</v>
       </c>
       <c r="C95" s="3">
         <v>6</v>
@@ -2751,8 +2738,8 @@
       <c r="A96" s="2">
         <v>2</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>6</v>
+      <c r="B96" s="2">
+        <v>4</v>
       </c>
       <c r="C96" s="3">
         <v>7</v>
@@ -2772,8 +2759,8 @@
       <c r="A97" s="2">
         <v>2</v>
       </c>
-      <c r="B97" s="2" t="s">
-        <v>6</v>
+      <c r="B97" s="2">
+        <v>4</v>
       </c>
       <c r="C97" s="3">
         <v>8</v>
@@ -2793,8 +2780,8 @@
       <c r="A98" s="4">
         <v>3</v>
       </c>
-      <c r="B98" s="4" t="s">
-        <v>3</v>
+      <c r="B98" s="4">
+        <v>1</v>
       </c>
       <c r="C98" s="5">
         <v>9</v>
@@ -2821,8 +2808,8 @@
       <c r="A99" s="4">
         <v>3</v>
       </c>
-      <c r="B99" s="4" t="s">
-        <v>3</v>
+      <c r="B99" s="4">
+        <v>1</v>
       </c>
       <c r="C99" s="5">
         <v>10</v>
@@ -2849,8 +2836,8 @@
       <c r="A100" s="4">
         <v>3</v>
       </c>
-      <c r="B100" s="4" t="s">
-        <v>3</v>
+      <c r="B100" s="4">
+        <v>1</v>
       </c>
       <c r="C100" s="5">
         <v>11</v>
@@ -2877,8 +2864,8 @@
       <c r="A101" s="4">
         <v>3</v>
       </c>
-      <c r="B101" s="4" t="s">
-        <v>3</v>
+      <c r="B101" s="4">
+        <v>1</v>
       </c>
       <c r="C101" s="5">
         <v>12</v>
@@ -2905,8 +2892,8 @@
       <c r="A102" s="4">
         <v>3</v>
       </c>
-      <c r="B102" s="4" t="s">
-        <v>4</v>
+      <c r="B102" s="4">
+        <v>2</v>
       </c>
       <c r="C102" s="5">
         <v>1</v>
@@ -2933,8 +2920,8 @@
       <c r="A103" s="4">
         <v>3</v>
       </c>
-      <c r="B103" s="4" t="s">
-        <v>5</v>
+      <c r="B103" s="4">
+        <v>3</v>
       </c>
       <c r="C103" s="5">
         <v>2</v>
@@ -2961,8 +2948,8 @@
       <c r="A104" s="4">
         <v>3</v>
       </c>
-      <c r="B104" s="4" t="s">
-        <v>5</v>
+      <c r="B104" s="4">
+        <v>3</v>
       </c>
       <c r="C104" s="5">
         <v>3</v>
@@ -2989,8 +2976,8 @@
       <c r="A105" s="4">
         <v>3</v>
       </c>
-      <c r="B105" s="4" t="s">
-        <v>5</v>
+      <c r="B105" s="4">
+        <v>3</v>
       </c>
       <c r="C105" s="5">
         <v>4</v>
@@ -3017,8 +3004,8 @@
       <c r="A106" s="4">
         <v>3</v>
       </c>
-      <c r="B106" s="4" t="s">
-        <v>5</v>
+      <c r="B106" s="4">
+        <v>3</v>
       </c>
       <c r="C106" s="5">
         <v>5</v>
@@ -3045,8 +3032,8 @@
       <c r="A107" s="4">
         <v>3</v>
       </c>
-      <c r="B107" s="4" t="s">
-        <v>6</v>
+      <c r="B107" s="4">
+        <v>4</v>
       </c>
       <c r="C107" s="5">
         <v>6</v>
@@ -3073,8 +3060,8 @@
       <c r="A108" s="4">
         <v>3</v>
       </c>
-      <c r="B108" s="4" t="s">
-        <v>6</v>
+      <c r="B108" s="4">
+        <v>4</v>
       </c>
       <c r="C108" s="5">
         <v>7</v>
@@ -3101,8 +3088,8 @@
       <c r="A109" s="4">
         <v>3</v>
       </c>
-      <c r="B109" s="4" t="s">
-        <v>6</v>
+      <c r="B109" s="4">
+        <v>4</v>
       </c>
       <c r="C109" s="5">
         <v>8</v>
@@ -3129,8 +3116,8 @@
       <c r="A110" s="2">
         <v>3</v>
       </c>
-      <c r="B110" s="2" t="s">
-        <v>3</v>
+      <c r="B110" s="2">
+        <v>1</v>
       </c>
       <c r="C110" s="3">
         <v>9</v>
@@ -3150,8 +3137,8 @@
       <c r="A111" s="2">
         <v>3</v>
       </c>
-      <c r="B111" s="2" t="s">
-        <v>3</v>
+      <c r="B111" s="2">
+        <v>1</v>
       </c>
       <c r="C111" s="3">
         <v>10</v>
@@ -3171,8 +3158,8 @@
       <c r="A112" s="2">
         <v>3</v>
       </c>
-      <c r="B112" s="2" t="s">
-        <v>3</v>
+      <c r="B112" s="2">
+        <v>1</v>
       </c>
       <c r="C112" s="3">
         <v>11</v>
@@ -3192,8 +3179,8 @@
       <c r="A113" s="2">
         <v>3</v>
       </c>
-      <c r="B113" s="2" t="s">
-        <v>3</v>
+      <c r="B113" s="2">
+        <v>1</v>
       </c>
       <c r="C113" s="3">
         <v>12</v>
@@ -3213,8 +3200,8 @@
       <c r="A114" s="2">
         <v>3</v>
       </c>
-      <c r="B114" s="2" t="s">
-        <v>4</v>
+      <c r="B114" s="2">
+        <v>2</v>
       </c>
       <c r="C114" s="3">
         <v>1</v>
@@ -3232,8 +3219,8 @@
       <c r="A115" s="2">
         <v>3</v>
       </c>
-      <c r="B115" s="2" t="s">
-        <v>5</v>
+      <c r="B115" s="2">
+        <v>3</v>
       </c>
       <c r="C115" s="3">
         <v>2</v>
@@ -3251,8 +3238,8 @@
       <c r="A116" s="2">
         <v>3</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>5</v>
+      <c r="B116" s="2">
+        <v>3</v>
       </c>
       <c r="C116" s="3">
         <v>3</v>
@@ -3270,8 +3257,8 @@
       <c r="A117" s="2">
         <v>3</v>
       </c>
-      <c r="B117" s="2" t="s">
-        <v>5</v>
+      <c r="B117" s="2">
+        <v>3</v>
       </c>
       <c r="C117" s="3">
         <v>4</v>
@@ -3289,8 +3276,8 @@
       <c r="A118" s="2">
         <v>3</v>
       </c>
-      <c r="B118" s="2" t="s">
-        <v>5</v>
+      <c r="B118" s="2">
+        <v>3</v>
       </c>
       <c r="C118" s="3">
         <v>5</v>
@@ -3308,8 +3295,8 @@
       <c r="A119" s="2">
         <v>3</v>
       </c>
-      <c r="B119" s="2" t="s">
-        <v>6</v>
+      <c r="B119" s="2">
+        <v>4</v>
       </c>
       <c r="C119" s="3">
         <v>6</v>
@@ -3327,8 +3314,8 @@
       <c r="A120" s="2">
         <v>3</v>
       </c>
-      <c r="B120" s="2" t="s">
-        <v>6</v>
+      <c r="B120" s="2">
+        <v>4</v>
       </c>
       <c r="C120" s="3">
         <v>7</v>
@@ -3346,8 +3333,8 @@
       <c r="A121" s="2">
         <v>3</v>
       </c>
-      <c r="B121" s="2" t="s">
-        <v>6</v>
+      <c r="B121" s="2">
+        <v>4</v>
       </c>
       <c r="C121" s="3">
         <v>8</v>
@@ -3365,8 +3352,8 @@
       <c r="A122" s="4">
         <v>3</v>
       </c>
-      <c r="B122" s="4" t="s">
-        <v>3</v>
+      <c r="B122" s="4">
+        <v>1</v>
       </c>
       <c r="C122" s="5">
         <v>9</v>
@@ -3384,8 +3371,8 @@
       <c r="A123" s="4">
         <v>3</v>
       </c>
-      <c r="B123" s="4" t="s">
-        <v>3</v>
+      <c r="B123" s="4">
+        <v>1</v>
       </c>
       <c r="C123" s="5">
         <v>10</v>
@@ -3403,8 +3390,8 @@
       <c r="A124" s="4">
         <v>3</v>
       </c>
-      <c r="B124" s="4" t="s">
-        <v>3</v>
+      <c r="B124" s="4">
+        <v>1</v>
       </c>
       <c r="C124" s="5">
         <v>11</v>
@@ -3422,8 +3409,8 @@
       <c r="A125" s="4">
         <v>3</v>
       </c>
-      <c r="B125" s="4" t="s">
-        <v>3</v>
+      <c r="B125" s="4">
+        <v>1</v>
       </c>
       <c r="C125" s="5">
         <v>12</v>
@@ -3441,8 +3428,8 @@
       <c r="A126" s="4">
         <v>3</v>
       </c>
-      <c r="B126" s="4" t="s">
-        <v>4</v>
+      <c r="B126" s="4">
+        <v>2</v>
       </c>
       <c r="C126" s="5">
         <v>1</v>
@@ -3462,8 +3449,8 @@
       <c r="A127" s="4">
         <v>3</v>
       </c>
-      <c r="B127" s="4" t="s">
-        <v>5</v>
+      <c r="B127" s="4">
+        <v>3</v>
       </c>
       <c r="C127" s="5">
         <v>2</v>
@@ -3483,8 +3470,8 @@
       <c r="A128" s="4">
         <v>3</v>
       </c>
-      <c r="B128" s="4" t="s">
-        <v>5</v>
+      <c r="B128" s="4">
+        <v>3</v>
       </c>
       <c r="C128" s="5">
         <v>3</v>
@@ -3504,8 +3491,8 @@
       <c r="A129" s="4">
         <v>3</v>
       </c>
-      <c r="B129" s="4" t="s">
-        <v>5</v>
+      <c r="B129" s="4">
+        <v>3</v>
       </c>
       <c r="C129" s="5">
         <v>4</v>
@@ -3525,8 +3512,8 @@
       <c r="A130" s="4">
         <v>3</v>
       </c>
-      <c r="B130" s="4" t="s">
-        <v>5</v>
+      <c r="B130" s="4">
+        <v>3</v>
       </c>
       <c r="C130" s="5">
         <v>5</v>
@@ -3546,8 +3533,8 @@
       <c r="A131" s="4">
         <v>3</v>
       </c>
-      <c r="B131" s="4" t="s">
-        <v>6</v>
+      <c r="B131" s="4">
+        <v>4</v>
       </c>
       <c r="C131" s="5">
         <v>6</v>
@@ -3567,8 +3554,8 @@
       <c r="A132" s="4">
         <v>3</v>
       </c>
-      <c r="B132" s="4" t="s">
-        <v>6</v>
+      <c r="B132" s="4">
+        <v>4</v>
       </c>
       <c r="C132" s="5">
         <v>7</v>
@@ -3588,8 +3575,8 @@
       <c r="A133" s="4">
         <v>3</v>
       </c>
-      <c r="B133" s="4" t="s">
-        <v>6</v>
+      <c r="B133" s="4">
+        <v>4</v>
       </c>
       <c r="C133" s="5">
         <v>8</v>
@@ -3609,8 +3596,8 @@
       <c r="A134" s="2">
         <v>3</v>
       </c>
-      <c r="B134" s="2" t="s">
-        <v>3</v>
+      <c r="B134" s="2">
+        <v>1</v>
       </c>
       <c r="C134" s="3">
         <v>9</v>
@@ -3630,8 +3617,8 @@
       <c r="A135" s="2">
         <v>3</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>3</v>
+      <c r="B135" s="2">
+        <v>1</v>
       </c>
       <c r="C135" s="3">
         <v>10</v>
@@ -3651,8 +3638,8 @@
       <c r="A136" s="2">
         <v>3</v>
       </c>
-      <c r="B136" s="2" t="s">
-        <v>3</v>
+      <c r="B136" s="2">
+        <v>1</v>
       </c>
       <c r="C136" s="3">
         <v>11</v>
@@ -3672,8 +3659,8 @@
       <c r="A137" s="2">
         <v>3</v>
       </c>
-      <c r="B137" s="2" t="s">
-        <v>3</v>
+      <c r="B137" s="2">
+        <v>1</v>
       </c>
       <c r="C137" s="3">
         <v>12</v>
@@ -3693,8 +3680,8 @@
       <c r="A138" s="2">
         <v>3</v>
       </c>
-      <c r="B138" s="2" t="s">
-        <v>4</v>
+      <c r="B138" s="2">
+        <v>2</v>
       </c>
       <c r="C138" s="3">
         <v>1</v>
@@ -3714,8 +3701,8 @@
       <c r="A139" s="2">
         <v>3</v>
       </c>
-      <c r="B139" s="2" t="s">
-        <v>5</v>
+      <c r="B139" s="2">
+        <v>3</v>
       </c>
       <c r="C139" s="3">
         <v>2</v>
@@ -3735,8 +3722,8 @@
       <c r="A140" s="2">
         <v>3</v>
       </c>
-      <c r="B140" s="2" t="s">
-        <v>5</v>
+      <c r="B140" s="2">
+        <v>3</v>
       </c>
       <c r="C140" s="3">
         <v>3</v>
@@ -3756,8 +3743,8 @@
       <c r="A141" s="2">
         <v>3</v>
       </c>
-      <c r="B141" s="2" t="s">
-        <v>5</v>
+      <c r="B141" s="2">
+        <v>3</v>
       </c>
       <c r="C141" s="3">
         <v>4</v>
@@ -3777,8 +3764,8 @@
       <c r="A142" s="2">
         <v>3</v>
       </c>
-      <c r="B142" s="2" t="s">
-        <v>5</v>
+      <c r="B142" s="2">
+        <v>3</v>
       </c>
       <c r="C142" s="3">
         <v>5</v>
@@ -3798,8 +3785,8 @@
       <c r="A143" s="2">
         <v>3</v>
       </c>
-      <c r="B143" s="2" t="s">
-        <v>6</v>
+      <c r="B143" s="2">
+        <v>4</v>
       </c>
       <c r="C143" s="3">
         <v>6</v>
@@ -3819,8 +3806,8 @@
       <c r="A144" s="2">
         <v>3</v>
       </c>
-      <c r="B144" s="2" t="s">
-        <v>6</v>
+      <c r="B144" s="2">
+        <v>4</v>
       </c>
       <c r="C144" s="3">
         <v>7</v>
@@ -3840,8 +3827,8 @@
       <c r="A145" s="2">
         <v>3</v>
       </c>
-      <c r="B145" s="2" t="s">
-        <v>6</v>
+      <c r="B145" s="2">
+        <v>4</v>
       </c>
       <c r="C145" s="3">
         <v>8</v>
@@ -3861,8 +3848,8 @@
       <c r="A146" s="4">
         <v>4</v>
       </c>
-      <c r="B146" s="4" t="s">
-        <v>3</v>
+      <c r="B146" s="4">
+        <v>1</v>
       </c>
       <c r="C146" s="5">
         <v>9</v>
@@ -3882,8 +3869,8 @@
       <c r="A147" s="4">
         <v>4</v>
       </c>
-      <c r="B147" s="4" t="s">
-        <v>3</v>
+      <c r="B147" s="4">
+        <v>1</v>
       </c>
       <c r="C147" s="5">
         <v>10</v>
@@ -3903,8 +3890,8 @@
       <c r="A148" s="4">
         <v>4</v>
       </c>
-      <c r="B148" s="4" t="s">
-        <v>3</v>
+      <c r="B148" s="4">
+        <v>1</v>
       </c>
       <c r="C148" s="5">
         <v>11</v>
@@ -3924,8 +3911,8 @@
       <c r="A149" s="4">
         <v>4</v>
       </c>
-      <c r="B149" s="4" t="s">
-        <v>3</v>
+      <c r="B149" s="4">
+        <v>1</v>
       </c>
       <c r="C149" s="5">
         <v>12</v>
@@ -3945,8 +3932,8 @@
       <c r="A150" s="4">
         <v>4</v>
       </c>
-      <c r="B150" s="4" t="s">
-        <v>4</v>
+      <c r="B150" s="4">
+        <v>2</v>
       </c>
       <c r="C150" s="5">
         <v>1</v>
@@ -3966,8 +3953,8 @@
       <c r="A151" s="4">
         <v>4</v>
       </c>
-      <c r="B151" s="4" t="s">
-        <v>5</v>
+      <c r="B151" s="4">
+        <v>3</v>
       </c>
       <c r="C151" s="5">
         <v>2</v>
@@ -3987,8 +3974,8 @@
       <c r="A152" s="4">
         <v>4</v>
       </c>
-      <c r="B152" s="4" t="s">
-        <v>5</v>
+      <c r="B152" s="4">
+        <v>3</v>
       </c>
       <c r="C152" s="5">
         <v>3</v>
@@ -4008,8 +3995,8 @@
       <c r="A153" s="4">
         <v>4</v>
       </c>
-      <c r="B153" s="4" t="s">
-        <v>5</v>
+      <c r="B153" s="4">
+        <v>3</v>
       </c>
       <c r="C153" s="5">
         <v>4</v>
@@ -4029,8 +4016,8 @@
       <c r="A154" s="4">
         <v>4</v>
       </c>
-      <c r="B154" s="4" t="s">
-        <v>5</v>
+      <c r="B154" s="4">
+        <v>3</v>
       </c>
       <c r="C154" s="5">
         <v>5</v>
@@ -4050,8 +4037,8 @@
       <c r="A155" s="4">
         <v>4</v>
       </c>
-      <c r="B155" s="4" t="s">
-        <v>6</v>
+      <c r="B155" s="4">
+        <v>4</v>
       </c>
       <c r="C155" s="5">
         <v>6</v>
@@ -4071,8 +4058,8 @@
       <c r="A156" s="4">
         <v>4</v>
       </c>
-      <c r="B156" s="4" t="s">
-        <v>6</v>
+      <c r="B156" s="4">
+        <v>4</v>
       </c>
       <c r="C156" s="5">
         <v>7</v>
@@ -4092,8 +4079,8 @@
       <c r="A157" s="4">
         <v>4</v>
       </c>
-      <c r="B157" s="4" t="s">
-        <v>6</v>
+      <c r="B157" s="4">
+        <v>4</v>
       </c>
       <c r="C157" s="5">
         <v>8</v>
@@ -4113,8 +4100,8 @@
       <c r="A158" s="2">
         <v>4</v>
       </c>
-      <c r="B158" s="2" t="s">
-        <v>3</v>
+      <c r="B158" s="2">
+        <v>1</v>
       </c>
       <c r="C158" s="3">
         <v>9</v>
@@ -4134,8 +4121,8 @@
       <c r="A159" s="2">
         <v>4</v>
       </c>
-      <c r="B159" s="2" t="s">
-        <v>3</v>
+      <c r="B159" s="2">
+        <v>1</v>
       </c>
       <c r="C159" s="3">
         <v>10</v>
@@ -4155,8 +4142,8 @@
       <c r="A160" s="2">
         <v>4</v>
       </c>
-      <c r="B160" s="2" t="s">
-        <v>3</v>
+      <c r="B160" s="2">
+        <v>1</v>
       </c>
       <c r="C160" s="3">
         <v>11</v>
@@ -4176,8 +4163,8 @@
       <c r="A161" s="2">
         <v>4</v>
       </c>
-      <c r="B161" s="2" t="s">
-        <v>3</v>
+      <c r="B161" s="2">
+        <v>1</v>
       </c>
       <c r="C161" s="3">
         <v>12</v>
@@ -4197,8 +4184,8 @@
       <c r="A162" s="2">
         <v>4</v>
       </c>
-      <c r="B162" s="2" t="s">
-        <v>4</v>
+      <c r="B162" s="2">
+        <v>2</v>
       </c>
       <c r="C162" s="3">
         <v>1</v>
@@ -4216,8 +4203,8 @@
       <c r="A163" s="2">
         <v>4</v>
       </c>
-      <c r="B163" s="2" t="s">
-        <v>5</v>
+      <c r="B163" s="2">
+        <v>3</v>
       </c>
       <c r="C163" s="3">
         <v>2</v>
@@ -4235,8 +4222,8 @@
       <c r="A164" s="2">
         <v>4</v>
       </c>
-      <c r="B164" s="2" t="s">
-        <v>5</v>
+      <c r="B164" s="2">
+        <v>3</v>
       </c>
       <c r="C164" s="3">
         <v>3</v>
@@ -4254,8 +4241,8 @@
       <c r="A165" s="2">
         <v>4</v>
       </c>
-      <c r="B165" s="2" t="s">
-        <v>5</v>
+      <c r="B165" s="2">
+        <v>3</v>
       </c>
       <c r="C165" s="3">
         <v>4</v>
@@ -4273,8 +4260,8 @@
       <c r="A166" s="2">
         <v>4</v>
       </c>
-      <c r="B166" s="2" t="s">
-        <v>5</v>
+      <c r="B166" s="2">
+        <v>3</v>
       </c>
       <c r="C166" s="3">
         <v>5</v>
@@ -4292,8 +4279,8 @@
       <c r="A167" s="2">
         <v>4</v>
       </c>
-      <c r="B167" s="2" t="s">
-        <v>6</v>
+      <c r="B167" s="2">
+        <v>4</v>
       </c>
       <c r="C167" s="3">
         <v>6</v>
@@ -4311,8 +4298,8 @@
       <c r="A168" s="2">
         <v>4</v>
       </c>
-      <c r="B168" s="2" t="s">
-        <v>6</v>
+      <c r="B168" s="2">
+        <v>4</v>
       </c>
       <c r="C168" s="3">
         <v>7</v>
@@ -4330,8 +4317,8 @@
       <c r="A169" s="2">
         <v>4</v>
       </c>
-      <c r="B169" s="2" t="s">
-        <v>6</v>
+      <c r="B169" s="2">
+        <v>4</v>
       </c>
       <c r="C169" s="3">
         <v>8</v>
@@ -4349,8 +4336,8 @@
       <c r="A170" s="4">
         <v>4</v>
       </c>
-      <c r="B170" s="4" t="s">
-        <v>3</v>
+      <c r="B170" s="4">
+        <v>1</v>
       </c>
       <c r="C170" s="5">
         <v>9</v>
@@ -4368,8 +4355,8 @@
       <c r="A171" s="4">
         <v>4</v>
       </c>
-      <c r="B171" s="4" t="s">
-        <v>3</v>
+      <c r="B171" s="4">
+        <v>1</v>
       </c>
       <c r="C171" s="5">
         <v>10</v>
@@ -4387,8 +4374,8 @@
       <c r="A172" s="4">
         <v>4</v>
       </c>
-      <c r="B172" s="4" t="s">
-        <v>3</v>
+      <c r="B172" s="4">
+        <v>1</v>
       </c>
       <c r="C172" s="5">
         <v>11</v>
@@ -4406,8 +4393,8 @@
       <c r="A173" s="4">
         <v>4</v>
       </c>
-      <c r="B173" s="4" t="s">
-        <v>3</v>
+      <c r="B173" s="4">
+        <v>1</v>
       </c>
       <c r="C173" s="5">
         <v>12</v>
@@ -4425,8 +4412,8 @@
       <c r="A174" s="4">
         <v>4</v>
       </c>
-      <c r="B174" s="4" t="s">
-        <v>4</v>
+      <c r="B174" s="4">
+        <v>2</v>
       </c>
       <c r="C174" s="5">
         <v>1</v>
@@ -4446,8 +4433,8 @@
       <c r="A175" s="4">
         <v>4</v>
       </c>
-      <c r="B175" s="4" t="s">
-        <v>5</v>
+      <c r="B175" s="4">
+        <v>3</v>
       </c>
       <c r="C175" s="5">
         <v>2</v>
@@ -4467,8 +4454,8 @@
       <c r="A176" s="4">
         <v>4</v>
       </c>
-      <c r="B176" s="4" t="s">
-        <v>5</v>
+      <c r="B176" s="4">
+        <v>3</v>
       </c>
       <c r="C176" s="5">
         <v>3</v>
@@ -4488,8 +4475,8 @@
       <c r="A177" s="4">
         <v>4</v>
       </c>
-      <c r="B177" s="4" t="s">
-        <v>5</v>
+      <c r="B177" s="4">
+        <v>3</v>
       </c>
       <c r="C177" s="5">
         <v>4</v>
@@ -4509,8 +4496,8 @@
       <c r="A178" s="4">
         <v>4</v>
       </c>
-      <c r="B178" s="4" t="s">
-        <v>5</v>
+      <c r="B178" s="4">
+        <v>3</v>
       </c>
       <c r="C178" s="5">
         <v>5</v>
@@ -4530,8 +4517,8 @@
       <c r="A179" s="4">
         <v>4</v>
       </c>
-      <c r="B179" s="4" t="s">
-        <v>6</v>
+      <c r="B179" s="4">
+        <v>4</v>
       </c>
       <c r="C179" s="5">
         <v>6</v>
@@ -4551,8 +4538,8 @@
       <c r="A180" s="4">
         <v>4</v>
       </c>
-      <c r="B180" s="4" t="s">
-        <v>6</v>
+      <c r="B180" s="4">
+        <v>4</v>
       </c>
       <c r="C180" s="5">
         <v>7</v>
@@ -4572,8 +4559,8 @@
       <c r="A181" s="4">
         <v>4</v>
       </c>
-      <c r="B181" s="4" t="s">
-        <v>6</v>
+      <c r="B181" s="4">
+        <v>4</v>
       </c>
       <c r="C181" s="5">
         <v>8</v>
@@ -4593,8 +4580,8 @@
       <c r="A182" s="2">
         <v>4</v>
       </c>
-      <c r="B182" s="2" t="s">
-        <v>3</v>
+      <c r="B182" s="2">
+        <v>1</v>
       </c>
       <c r="C182" s="3">
         <v>9</v>
@@ -4614,8 +4601,8 @@
       <c r="A183" s="2">
         <v>4</v>
       </c>
-      <c r="B183" s="2" t="s">
-        <v>3</v>
+      <c r="B183" s="2">
+        <v>1</v>
       </c>
       <c r="C183" s="3">
         <v>10</v>
@@ -4635,8 +4622,8 @@
       <c r="A184" s="2">
         <v>4</v>
       </c>
-      <c r="B184" s="2" t="s">
-        <v>3</v>
+      <c r="B184" s="2">
+        <v>1</v>
       </c>
       <c r="C184" s="3">
         <v>11</v>
@@ -4656,8 +4643,8 @@
       <c r="A185" s="2">
         <v>4</v>
       </c>
-      <c r="B185" s="2" t="s">
-        <v>3</v>
+      <c r="B185" s="2">
+        <v>1</v>
       </c>
       <c r="C185" s="3">
         <v>12</v>
@@ -4677,8 +4664,8 @@
       <c r="A186" s="2">
         <v>4</v>
       </c>
-      <c r="B186" s="2" t="s">
-        <v>4</v>
+      <c r="B186" s="2">
+        <v>2</v>
       </c>
       <c r="C186" s="3">
         <v>1</v>
@@ -4698,8 +4685,8 @@
       <c r="A187" s="2">
         <v>4</v>
       </c>
-      <c r="B187" s="2" t="s">
-        <v>5</v>
+      <c r="B187" s="2">
+        <v>3</v>
       </c>
       <c r="C187" s="3">
         <v>2</v>
@@ -4719,8 +4706,8 @@
       <c r="A188" s="2">
         <v>4</v>
       </c>
-      <c r="B188" s="2" t="s">
-        <v>5</v>
+      <c r="B188" s="2">
+        <v>3</v>
       </c>
       <c r="C188" s="3">
         <v>3</v>
@@ -4740,8 +4727,8 @@
       <c r="A189" s="2">
         <v>4</v>
       </c>
-      <c r="B189" s="2" t="s">
-        <v>5</v>
+      <c r="B189" s="2">
+        <v>3</v>
       </c>
       <c r="C189" s="3">
         <v>4</v>
@@ -4761,8 +4748,8 @@
       <c r="A190" s="2">
         <v>4</v>
       </c>
-      <c r="B190" s="2" t="s">
-        <v>5</v>
+      <c r="B190" s="2">
+        <v>3</v>
       </c>
       <c r="C190" s="3">
         <v>5</v>
@@ -4782,8 +4769,8 @@
       <c r="A191" s="2">
         <v>4</v>
       </c>
-      <c r="B191" s="2" t="s">
-        <v>6</v>
+      <c r="B191" s="2">
+        <v>4</v>
       </c>
       <c r="C191" s="3">
         <v>6</v>
@@ -4803,8 +4790,8 @@
       <c r="A192" s="2">
         <v>4</v>
       </c>
-      <c r="B192" s="2" t="s">
-        <v>6</v>
+      <c r="B192" s="2">
+        <v>4</v>
       </c>
       <c r="C192" s="3">
         <v>7</v>
@@ -4824,8 +4811,8 @@
       <c r="A193" s="2">
         <v>4</v>
       </c>
-      <c r="B193" s="2" t="s">
-        <v>6</v>
+      <c r="B193" s="2">
+        <v>4</v>
       </c>
       <c r="C193" s="3">
         <v>8</v>
@@ -4845,8 +4832,8 @@
       <c r="A194" s="4">
         <v>5</v>
       </c>
-      <c r="B194" s="4" t="s">
-        <v>3</v>
+      <c r="B194" s="4">
+        <v>1</v>
       </c>
       <c r="C194" s="5">
         <v>9</v>
@@ -4866,8 +4853,8 @@
       <c r="A195" s="4">
         <v>5</v>
       </c>
-      <c r="B195" s="4" t="s">
-        <v>3</v>
+      <c r="B195" s="4">
+        <v>1</v>
       </c>
       <c r="C195" s="5">
         <v>10</v>
@@ -4887,8 +4874,8 @@
       <c r="A196" s="4">
         <v>5</v>
       </c>
-      <c r="B196" s="4" t="s">
-        <v>3</v>
+      <c r="B196" s="4">
+        <v>1</v>
       </c>
       <c r="C196" s="5">
         <v>11</v>
@@ -4908,8 +4895,8 @@
       <c r="A197" s="4">
         <v>5</v>
       </c>
-      <c r="B197" s="4" t="s">
-        <v>3</v>
+      <c r="B197" s="4">
+        <v>1</v>
       </c>
       <c r="C197" s="5">
         <v>12</v>
@@ -4929,8 +4916,8 @@
       <c r="A198" s="4">
         <v>5</v>
       </c>
-      <c r="B198" s="4" t="s">
-        <v>4</v>
+      <c r="B198" s="4">
+        <v>2</v>
       </c>
       <c r="C198" s="5">
         <v>1</v>
@@ -4950,8 +4937,8 @@
       <c r="A199" s="4">
         <v>5</v>
       </c>
-      <c r="B199" s="4" t="s">
-        <v>5</v>
+      <c r="B199" s="4">
+        <v>3</v>
       </c>
       <c r="C199" s="5">
         <v>2</v>
@@ -4971,8 +4958,8 @@
       <c r="A200" s="4">
         <v>5</v>
       </c>
-      <c r="B200" s="4" t="s">
-        <v>5</v>
+      <c r="B200" s="4">
+        <v>3</v>
       </c>
       <c r="C200" s="5">
         <v>3</v>
@@ -4992,8 +4979,8 @@
       <c r="A201" s="4">
         <v>5</v>
       </c>
-      <c r="B201" s="4" t="s">
-        <v>5</v>
+      <c r="B201" s="4">
+        <v>3</v>
       </c>
       <c r="C201" s="5">
         <v>4</v>
@@ -5013,8 +5000,8 @@
       <c r="A202" s="4">
         <v>5</v>
       </c>
-      <c r="B202" s="4" t="s">
-        <v>5</v>
+      <c r="B202" s="4">
+        <v>3</v>
       </c>
       <c r="C202" s="5">
         <v>5</v>
@@ -5034,8 +5021,8 @@
       <c r="A203" s="4">
         <v>5</v>
       </c>
-      <c r="B203" s="4" t="s">
-        <v>6</v>
+      <c r="B203" s="4">
+        <v>4</v>
       </c>
       <c r="C203" s="5">
         <v>6</v>
@@ -5055,8 +5042,8 @@
       <c r="A204" s="4">
         <v>5</v>
       </c>
-      <c r="B204" s="4" t="s">
-        <v>6</v>
+      <c r="B204" s="4">
+        <v>4</v>
       </c>
       <c r="C204" s="5">
         <v>7</v>
@@ -5076,8 +5063,8 @@
       <c r="A205" s="4">
         <v>5</v>
       </c>
-      <c r="B205" s="4" t="s">
-        <v>6</v>
+      <c r="B205" s="4">
+        <v>4</v>
       </c>
       <c r="C205" s="5">
         <v>8</v>
@@ -5097,8 +5084,8 @@
       <c r="A206" s="2">
         <v>5</v>
       </c>
-      <c r="B206" s="2" t="s">
-        <v>3</v>
+      <c r="B206" s="2">
+        <v>1</v>
       </c>
       <c r="C206" s="3">
         <v>9</v>
@@ -5118,8 +5105,8 @@
       <c r="A207" s="2">
         <v>5</v>
       </c>
-      <c r="B207" s="2" t="s">
-        <v>3</v>
+      <c r="B207" s="2">
+        <v>1</v>
       </c>
       <c r="C207" s="3">
         <v>10</v>
@@ -5139,8 +5126,8 @@
       <c r="A208" s="2">
         <v>5</v>
       </c>
-      <c r="B208" s="2" t="s">
-        <v>3</v>
+      <c r="B208" s="2">
+        <v>1</v>
       </c>
       <c r="C208" s="3">
         <v>11</v>
@@ -5160,8 +5147,8 @@
       <c r="A209" s="2">
         <v>5</v>
       </c>
-      <c r="B209" s="2" t="s">
-        <v>3</v>
+      <c r="B209" s="2">
+        <v>1</v>
       </c>
       <c r="C209" s="3">
         <v>12</v>
@@ -5181,8 +5168,8 @@
       <c r="A210" s="2">
         <v>5</v>
       </c>
-      <c r="B210" s="2" t="s">
-        <v>4</v>
+      <c r="B210" s="2">
+        <v>2</v>
       </c>
       <c r="C210" s="3">
         <v>1</v>
@@ -5200,8 +5187,8 @@
       <c r="A211" s="2">
         <v>5</v>
       </c>
-      <c r="B211" s="2" t="s">
-        <v>5</v>
+      <c r="B211" s="2">
+        <v>3</v>
       </c>
       <c r="C211" s="3">
         <v>2</v>
@@ -5219,8 +5206,8 @@
       <c r="A212" s="2">
         <v>5</v>
       </c>
-      <c r="B212" s="2" t="s">
-        <v>5</v>
+      <c r="B212" s="2">
+        <v>3</v>
       </c>
       <c r="C212" s="3">
         <v>3</v>
@@ -5238,8 +5225,8 @@
       <c r="A213" s="2">
         <v>5</v>
       </c>
-      <c r="B213" s="2" t="s">
-        <v>5</v>
+      <c r="B213" s="2">
+        <v>3</v>
       </c>
       <c r="C213" s="3">
         <v>4</v>
@@ -5257,8 +5244,8 @@
       <c r="A214" s="2">
         <v>5</v>
       </c>
-      <c r="B214" s="2" t="s">
-        <v>5</v>
+      <c r="B214" s="2">
+        <v>3</v>
       </c>
       <c r="C214" s="3">
         <v>5</v>
@@ -5276,8 +5263,8 @@
       <c r="A215" s="2">
         <v>5</v>
       </c>
-      <c r="B215" s="2" t="s">
-        <v>6</v>
+      <c r="B215" s="2">
+        <v>4</v>
       </c>
       <c r="C215" s="3">
         <v>6</v>
@@ -5295,8 +5282,8 @@
       <c r="A216" s="2">
         <v>5</v>
       </c>
-      <c r="B216" s="2" t="s">
-        <v>6</v>
+      <c r="B216" s="2">
+        <v>4</v>
       </c>
       <c r="C216" s="3">
         <v>7</v>
@@ -5314,8 +5301,8 @@
       <c r="A217" s="2">
         <v>5</v>
       </c>
-      <c r="B217" s="2" t="s">
-        <v>6</v>
+      <c r="B217" s="2">
+        <v>4</v>
       </c>
       <c r="C217" s="3">
         <v>8</v>
@@ -5333,8 +5320,8 @@
       <c r="A218" s="4">
         <v>5</v>
       </c>
-      <c r="B218" s="4" t="s">
-        <v>3</v>
+      <c r="B218" s="4">
+        <v>1</v>
       </c>
       <c r="C218" s="5">
         <v>9</v>
@@ -5352,8 +5339,8 @@
       <c r="A219" s="4">
         <v>5</v>
       </c>
-      <c r="B219" s="4" t="s">
-        <v>3</v>
+      <c r="B219" s="4">
+        <v>1</v>
       </c>
       <c r="C219" s="5">
         <v>10</v>
@@ -5371,8 +5358,8 @@
       <c r="A220" s="4">
         <v>5</v>
       </c>
-      <c r="B220" s="4" t="s">
-        <v>3</v>
+      <c r="B220" s="4">
+        <v>1</v>
       </c>
       <c r="C220" s="5">
         <v>11</v>
@@ -5390,8 +5377,8 @@
       <c r="A221" s="4">
         <v>5</v>
       </c>
-      <c r="B221" s="4" t="s">
-        <v>3</v>
+      <c r="B221" s="4">
+        <v>1</v>
       </c>
       <c r="C221" s="5">
         <v>12</v>
@@ -5409,8 +5396,8 @@
       <c r="A222" s="4">
         <v>5</v>
       </c>
-      <c r="B222" s="4" t="s">
-        <v>4</v>
+      <c r="B222" s="4">
+        <v>2</v>
       </c>
       <c r="C222" s="5">
         <v>1</v>
@@ -5430,8 +5417,8 @@
       <c r="A223" s="4">
         <v>5</v>
       </c>
-      <c r="B223" s="4" t="s">
-        <v>5</v>
+      <c r="B223" s="4">
+        <v>3</v>
       </c>
       <c r="C223" s="5">
         <v>2</v>
@@ -5451,8 +5438,8 @@
       <c r="A224" s="4">
         <v>5</v>
       </c>
-      <c r="B224" s="4" t="s">
-        <v>5</v>
+      <c r="B224" s="4">
+        <v>3</v>
       </c>
       <c r="C224" s="5">
         <v>3</v>
@@ -5472,8 +5459,8 @@
       <c r="A225" s="4">
         <v>5</v>
       </c>
-      <c r="B225" s="4" t="s">
-        <v>5</v>
+      <c r="B225" s="4">
+        <v>3</v>
       </c>
       <c r="C225" s="5">
         <v>4</v>
@@ -5493,8 +5480,8 @@
       <c r="A226" s="4">
         <v>5</v>
       </c>
-      <c r="B226" s="4" t="s">
-        <v>5</v>
+      <c r="B226" s="4">
+        <v>3</v>
       </c>
       <c r="C226" s="5">
         <v>5</v>
@@ -5514,8 +5501,8 @@
       <c r="A227" s="4">
         <v>5</v>
       </c>
-      <c r="B227" s="4" t="s">
-        <v>6</v>
+      <c r="B227" s="4">
+        <v>4</v>
       </c>
       <c r="C227" s="5">
         <v>6</v>
@@ -5535,8 +5522,8 @@
       <c r="A228" s="4">
         <v>5</v>
       </c>
-      <c r="B228" s="4" t="s">
-        <v>6</v>
+      <c r="B228" s="4">
+        <v>4</v>
       </c>
       <c r="C228" s="5">
         <v>7</v>
@@ -5556,8 +5543,8 @@
       <c r="A229" s="4">
         <v>5</v>
       </c>
-      <c r="B229" s="4" t="s">
-        <v>6</v>
+      <c r="B229" s="4">
+        <v>4</v>
       </c>
       <c r="C229" s="5">
         <v>8</v>
@@ -5577,8 +5564,8 @@
       <c r="A230" s="2">
         <v>5</v>
       </c>
-      <c r="B230" s="2" t="s">
-        <v>3</v>
+      <c r="B230" s="2">
+        <v>1</v>
       </c>
       <c r="C230" s="3">
         <v>9</v>
@@ -5598,8 +5585,8 @@
       <c r="A231" s="2">
         <v>5</v>
       </c>
-      <c r="B231" s="2" t="s">
-        <v>3</v>
+      <c r="B231" s="2">
+        <v>1</v>
       </c>
       <c r="C231" s="3">
         <v>10</v>
@@ -5619,8 +5606,8 @@
       <c r="A232" s="2">
         <v>5</v>
       </c>
-      <c r="B232" s="2" t="s">
-        <v>3</v>
+      <c r="B232" s="2">
+        <v>1</v>
       </c>
       <c r="C232" s="3">
         <v>11</v>
@@ -5640,8 +5627,8 @@
       <c r="A233" s="2">
         <v>5</v>
       </c>
-      <c r="B233" s="2" t="s">
-        <v>3</v>
+      <c r="B233" s="2">
+        <v>1</v>
       </c>
       <c r="C233" s="3">
         <v>12</v>
@@ -5661,8 +5648,8 @@
       <c r="A234" s="2">
         <v>5</v>
       </c>
-      <c r="B234" s="2" t="s">
-        <v>4</v>
+      <c r="B234" s="2">
+        <v>2</v>
       </c>
       <c r="C234" s="3">
         <v>1</v>
@@ -5682,8 +5669,8 @@
       <c r="A235" s="2">
         <v>5</v>
       </c>
-      <c r="B235" s="2" t="s">
-        <v>5</v>
+      <c r="B235" s="2">
+        <v>3</v>
       </c>
       <c r="C235" s="3">
         <v>2</v>
@@ -5703,8 +5690,8 @@
       <c r="A236" s="2">
         <v>5</v>
       </c>
-      <c r="B236" s="2" t="s">
-        <v>5</v>
+      <c r="B236" s="2">
+        <v>3</v>
       </c>
       <c r="C236" s="3">
         <v>3</v>
@@ -5724,8 +5711,8 @@
       <c r="A237" s="2">
         <v>5</v>
       </c>
-      <c r="B237" s="2" t="s">
-        <v>5</v>
+      <c r="B237" s="2">
+        <v>3</v>
       </c>
       <c r="C237" s="3">
         <v>4</v>
@@ -5745,8 +5732,8 @@
       <c r="A238" s="2">
         <v>5</v>
       </c>
-      <c r="B238" s="2" t="s">
-        <v>5</v>
+      <c r="B238" s="2">
+        <v>3</v>
       </c>
       <c r="C238" s="3">
         <v>5</v>
@@ -5766,8 +5753,8 @@
       <c r="A239" s="2">
         <v>5</v>
       </c>
-      <c r="B239" s="2" t="s">
-        <v>6</v>
+      <c r="B239" s="2">
+        <v>4</v>
       </c>
       <c r="C239" s="3">
         <v>6</v>
@@ -5787,8 +5774,8 @@
       <c r="A240" s="2">
         <v>5</v>
       </c>
-      <c r="B240" s="2" t="s">
-        <v>6</v>
+      <c r="B240" s="2">
+        <v>4</v>
       </c>
       <c r="C240" s="3">
         <v>7</v>
@@ -5808,8 +5795,8 @@
       <c r="A241" s="2">
         <v>5</v>
       </c>
-      <c r="B241" s="2" t="s">
-        <v>6</v>
+      <c r="B241" s="2">
+        <v>4</v>
       </c>
       <c r="C241" s="3">
         <v>8</v>

</xml_diff>

<commit_message>
Data Pred for next year
</commit_message>
<xml_diff>
--- a/DinningData.xlsx
+++ b/DinningData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m.mughees/Desktop/DailyHours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F015619-58A3-884A-86A1-DB15764A0919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720CC216-5520-A642-BDDF-199D9BFD7B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{DE998561-EBAC-6C45-B2D5-E0BAD589018C}"/>
+    <workbookView xWindow="-19180" yWindow="-23680" windowWidth="28800" windowHeight="16260" activeTab="1" xr2:uid="{DE998561-EBAC-6C45-B2D5-E0BAD589018C}"/>
   </bookViews>
   <sheets>
     <sheet name="Cleaned Data" sheetId="1" r:id="rId1"/>
@@ -6070,8 +6070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED2650A-6E4F-6D49-92A6-976CF649E6D8}">
   <dimension ref="A1:T286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
+      <selection activeCell="I280" sqref="I280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
all updated charts added for per yer
</commit_message>
<xml_diff>
--- a/DinningData.xlsx
+++ b/DinningData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m.mughees/Desktop/DailyHours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BDDE47-BB4E-3D47-9BC6-263DFF2BE133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AABCCA3-2EE4-3548-8581-93C6846ECD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20000" yWindow="-26860" windowWidth="24080" windowHeight="18880" xr2:uid="{DE998561-EBAC-6C45-B2D5-E0BAD589018C}"/>
   </bookViews>
@@ -615,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9694C3E-4676-5E45-83AA-01CD38B8296E}">
   <dimension ref="A1:T241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added new code for data prediction
</commit_message>
<xml_diff>
--- a/DinningData.xlsx
+++ b/DinningData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m.mughees/Desktop/DailyHours/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AABCCA3-2EE4-3548-8581-93C6846ECD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464618B8-055F-4244-B528-88EB1CC2EC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20000" yWindow="-26860" windowWidth="24080" windowHeight="18880" xr2:uid="{DE998561-EBAC-6C45-B2D5-E0BAD589018C}"/>
+    <workbookView xWindow="-20000" yWindow="-26860" windowWidth="24080" windowHeight="18880" activeTab="1" xr2:uid="{DE998561-EBAC-6C45-B2D5-E0BAD589018C}"/>
   </bookViews>
   <sheets>
     <sheet name="Cleaned Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Data for 2025 pred" sheetId="3" r:id="rId2"/>
-    <sheet name="Data for Linear" sheetId="2" r:id="rId3"/>
+    <sheet name="Academic Year 24 25 " sheetId="4" r:id="rId2"/>
+    <sheet name="Data for 2025 pred" sheetId="3" r:id="rId3"/>
+    <sheet name="Data for Linear" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="33">
   <si>
     <t>DEP</t>
   </si>
@@ -135,6 +136,9 @@
   <si>
     <t>Academic Year</t>
   </si>
+  <si>
+    <t>24/25</t>
+  </si>
 </sst>
 </file>
 
@@ -143,7 +147,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,6 +204,22 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="Roboto Slab"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -224,10 +244,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -279,8 +300,22 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -615,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9694C3E-4676-5E45-83AA-01CD38B8296E}">
   <dimension ref="A1:T241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A184" workbookViewId="0">
+      <selection activeCell="A194" sqref="A194:C202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.2"/>
@@ -6025,11 +6060,1000 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E54AECD-9AF1-F944-B262-8AF2679566A9}">
+  <dimension ref="A1:F46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="12">
+        <v>1461.1375</v>
+      </c>
+      <c r="F2" s="21">
+        <f>E2*9.25</f>
+        <v>13515.521875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1461.1375</v>
+      </c>
+      <c r="F3" s="21">
+        <f t="shared" ref="F3:F10" si="0">E3*9.25</f>
+        <v>13515.521875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="12">
+        <v>956.5625</v>
+      </c>
+      <c r="F4" s="21">
+        <f t="shared" si="0"/>
+        <v>8848.203125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="12">
+        <v>993.36749999999995</v>
+      </c>
+      <c r="F5" s="21">
+        <f t="shared" si="0"/>
+        <v>9188.6493749999991</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="12">
+        <v>896.55250000000001</v>
+      </c>
+      <c r="F6" s="21">
+        <f t="shared" si="0"/>
+        <v>8293.1106249999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="12">
+        <v>797.36249999999995</v>
+      </c>
+      <c r="F7" s="21">
+        <f t="shared" si="0"/>
+        <v>7375.6031249999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="12">
+        <v>839.66499999999996</v>
+      </c>
+      <c r="F8" s="21">
+        <f t="shared" si="0"/>
+        <v>7766.9012499999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="12">
+        <v>756.66</v>
+      </c>
+      <c r="F9" s="21">
+        <f t="shared" si="0"/>
+        <v>6999.1049999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="12">
+        <v>665.70749999999998</v>
+      </c>
+      <c r="F10" s="21">
+        <f t="shared" si="0"/>
+        <v>6157.7943749999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="13">
+        <v>1170.6524999999999</v>
+      </c>
+      <c r="F11" s="22">
+        <f>E11*9.25</f>
+        <v>10828.535624999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1082.915</v>
+      </c>
+      <c r="F12" s="22">
+        <f t="shared" ref="F12:F19" si="1">E12*9.25</f>
+        <v>10016.963749999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="13">
+        <v>590.89250000000004</v>
+      </c>
+      <c r="F13" s="22">
+        <f t="shared" si="1"/>
+        <v>5465.7556250000007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="13">
+        <v>459.15499999999997</v>
+      </c>
+      <c r="F14" s="22">
+        <f t="shared" si="1"/>
+        <v>4247.1837500000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="13">
+        <v>701.2</v>
+      </c>
+      <c r="F15" s="22">
+        <f t="shared" si="1"/>
+        <v>6486.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="13">
+        <v>747.45</v>
+      </c>
+      <c r="F16" s="22">
+        <f t="shared" si="1"/>
+        <v>6913.9125000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="13">
+        <v>613.34749999999997</v>
+      </c>
+      <c r="F17" s="22">
+        <f t="shared" si="1"/>
+        <v>5673.4643749999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="13">
+        <v>536.59</v>
+      </c>
+      <c r="F18" s="22">
+        <f t="shared" si="1"/>
+        <v>4963.4575000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="13">
+        <v>451.10750000000002</v>
+      </c>
+      <c r="F19" s="22">
+        <f t="shared" si="1"/>
+        <v>4172.7443750000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" s="12">
+        <v>634.73749999999995</v>
+      </c>
+      <c r="F20" s="21">
+        <f>E20*9.25</f>
+        <v>5871.3218749999996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" s="12">
+        <v>589.625</v>
+      </c>
+      <c r="F21" s="21">
+        <f t="shared" ref="F21:F28" si="2">E21*9.25</f>
+        <v>5454.03125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="12">
+        <v>382.70249999999999</v>
+      </c>
+      <c r="F22" s="21">
+        <f t="shared" si="2"/>
+        <v>3539.9981250000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E23" s="12">
+        <v>310.88499999999999</v>
+      </c>
+      <c r="F23" s="21">
+        <f t="shared" si="2"/>
+        <v>2875.6862499999997</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="12">
+        <v>413.35</v>
+      </c>
+      <c r="F24" s="21">
+        <f t="shared" si="2"/>
+        <v>3823.4875000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="12">
+        <v>463.94</v>
+      </c>
+      <c r="F25" s="21">
+        <f t="shared" si="2"/>
+        <v>4291.4449999999997</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E26" s="12">
+        <v>375.08249999999998</v>
+      </c>
+      <c r="F26" s="21">
+        <f t="shared" si="2"/>
+        <v>3469.5131249999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="12">
+        <v>450.8175</v>
+      </c>
+      <c r="F27" s="21">
+        <f t="shared" si="2"/>
+        <v>4170.0618750000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E28" s="12">
+        <v>263.91500000000002</v>
+      </c>
+      <c r="F28" s="21">
+        <f t="shared" si="2"/>
+        <v>2441.2137500000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E29" s="13">
+        <v>431.9325</v>
+      </c>
+      <c r="F29" s="22">
+        <f>E29*9.25</f>
+        <v>3995.3756250000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="13">
+        <v>326.72750000000002</v>
+      </c>
+      <c r="F30" s="22">
+        <f t="shared" ref="F30:F37" si="3">E30*9.25</f>
+        <v>3022.2293750000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" s="13">
+        <v>339.54500000000002</v>
+      </c>
+      <c r="F31" s="22">
+        <f t="shared" si="3"/>
+        <v>3140.7912500000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E32" s="13">
+        <v>251.55500000000001</v>
+      </c>
+      <c r="F32" s="22">
+        <f t="shared" si="3"/>
+        <v>2326.88375</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="13">
+        <v>250.1525</v>
+      </c>
+      <c r="F33" s="22">
+        <f t="shared" si="3"/>
+        <v>2313.910625</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E34" s="13">
+        <v>289.49250000000001</v>
+      </c>
+      <c r="F34" s="22">
+        <f t="shared" si="3"/>
+        <v>2677.805625</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="13">
+        <v>188.76249999999999</v>
+      </c>
+      <c r="F35" s="22">
+        <f t="shared" si="3"/>
+        <v>1746.0531249999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="13">
+        <v>216.03749999999999</v>
+      </c>
+      <c r="F36" s="22">
+        <f t="shared" si="3"/>
+        <v>1998.346875</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="E37" s="13">
+        <v>139.97749999999999</v>
+      </c>
+      <c r="F37" s="22">
+        <f t="shared" si="3"/>
+        <v>1294.7918749999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="12">
+        <v>255.55333300000001</v>
+      </c>
+      <c r="F38" s="21">
+        <f>E38*9.25</f>
+        <v>2363.8683302499999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E39" s="12">
+        <v>256.97791699999999</v>
+      </c>
+      <c r="F39" s="21">
+        <f t="shared" ref="F39:F46" si="4">E39*9.25</f>
+        <v>2377.0457322500001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" s="12">
+        <v>173.52500000000001</v>
+      </c>
+      <c r="F40" s="21">
+        <f t="shared" si="4"/>
+        <v>1605.10625</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E41" s="12">
+        <v>180.67375000000001</v>
+      </c>
+      <c r="F41" s="21">
+        <f t="shared" si="4"/>
+        <v>1671.2321875</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" s="12">
+        <v>135.2225</v>
+      </c>
+      <c r="F42" s="21">
+        <f t="shared" si="4"/>
+        <v>1250.808125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43" s="12">
+        <v>114.84</v>
+      </c>
+      <c r="F43" s="21">
+        <f t="shared" si="4"/>
+        <v>1062.27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="12">
+        <v>125.68</v>
+      </c>
+      <c r="F44" s="21">
+        <f t="shared" si="4"/>
+        <v>1162.54</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="12">
+        <v>122.97499999999999</v>
+      </c>
+      <c r="F45" s="21">
+        <f t="shared" si="4"/>
+        <v>1137.51875</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="22" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="12">
+        <v>88.197500000000005</v>
+      </c>
+      <c r="F46" s="21">
+        <f t="shared" si="4"/>
+        <v>815.82687500000009</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ED2650A-6E4F-6D49-92A6-976CF649E6D8}">
   <dimension ref="A1:T286"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I222" sqref="I222"/>
+    <sheetView topLeftCell="A267" workbookViewId="0">
+      <selection activeCell="E278" sqref="E278:E286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.2"/>
@@ -12381,7 +13405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7D9360-6883-914F-8D66-A3A767BBCBBF}">
   <dimension ref="A1:T241"/>
   <sheetViews>

</xml_diff>